<commit_message>
feat: Realizando trade Rise/Fall
</commit_message>
<xml_diff>
--- a/Tokens_DEMO.xlsx
+++ b/Tokens_DEMO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PEDRO\Documents\Programacao\C#\Desktop\DEMO.app.deriv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F3D470D-CED8-4602-9A8A-4DB4F7A39D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884439FF-93F9-4533-9416-D2B4C78F5CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1155" windowWidth="18000" windowHeight="9360" xr2:uid="{1CD1A957-21DF-45E7-BB84-F2956879E42E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1CD1A957-21DF-45E7-BB84-F2956879E42E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Ler</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>demo_teste</t>
+  </si>
+  <si>
+    <t>full_teste</t>
+  </si>
+  <si>
+    <t>5a7J4zG40xIUAZe</t>
   </si>
 </sst>
 </file>
@@ -204,9 +210,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -217,9 +220,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -236,6 +236,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72932EC-1D0F-424D-8DBA-649E2BE102D8}">
-  <dimension ref="D1:J8"/>
+  <dimension ref="D1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -570,108 +576,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="4:10" s="14" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="10" t="s">
+    <row r="2" spans="4:10" s="12" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="11">
         <v>66069</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="4" spans="4:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="4:10" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="7" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="7" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="7" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>